<commit_message>
Demand Dataframe and Plots
Plots to be updated tomorrow
</commit_message>
<xml_diff>
--- a/1 - Scenario Processing/Annual Service Area Demand Scenarios/Output/MI.xlsx
+++ b/1 - Scenario Processing/Annual Service Area Demand Scenarios/Output/MI.xlsx
@@ -23,22 +23,22 @@
     <t xml:space="preserve">MI_SA_PCDD_2015</t>
   </si>
   <si>
-    <t xml:space="preserve">MI_SA_ETInc_2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDec_ETInc_2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDD_ETInc_2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_ETDec_2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDec_ETDec_2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDD_ETDec_2015</t>
+    <t xml:space="preserve">MI_SA_ET15_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDec_ET15_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDD_ET15_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_ETLow_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDec_ETLow_2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDD_ETLow_2015</t>
   </si>
   <si>
     <t xml:space="preserve">MI_SA_2070</t>
@@ -50,22 +50,22 @@
     <t xml:space="preserve">MI_SA_PCDD_2070</t>
   </si>
   <si>
-    <t xml:space="preserve">MI_SA_ETInc_2070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDec_ETInc_2070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDD_ETInc_2070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_ETDec_2070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDec_ETDec_2070</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDD_ETDec_2070</t>
+    <t xml:space="preserve">MI_SA_ET15_2070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDec_ET15_2070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDD_ET15_2070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_ETLow_2070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDec_ETLow_2070</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDD_ETLow_2070</t>
   </si>
   <si>
     <t xml:space="preserve">MI_SA_2150</t>
@@ -77,22 +77,22 @@
     <t xml:space="preserve">MI_SA_PCDD_2150</t>
   </si>
   <si>
-    <t xml:space="preserve">MI_SA_ETInc_2150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDec_ETInc_2150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDD_ETInc_2150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_ETDec_2150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDec_ETDec_2150</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MI_SA_PCDD_ETDec_2150</t>
+    <t xml:space="preserve">MI_SA_ET15_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDec_ET15_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDD_ET15_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_ETLow_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDec_ETLow_2150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MI_SA_PCDD_ETLow_2150</t>
   </si>
 </sst>
 </file>

</xml_diff>